<commit_message>
added navigation between worlds
</commit_message>
<xml_diff>
--- a/darkworld/model/data/floor builder 20200330.xlsx
+++ b/darkworld/model/data/floor builder 20200330.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Development\Python\DarkWorld\darkworld\model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA717EB3-4D97-40CF-B4E6-3B42C7240993}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224439F3-F6D4-4573-9365-152892B8B16C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="4140" windowWidth="28800" windowHeight="15840" tabRatio="904" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15240" yWindow="3795" windowWidth="28800" windowHeight="15840" tabRatio="904" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reverser" sheetId="33" r:id="rId1"/>
     <sheet name="Blank" sheetId="49" r:id="rId2"/>
     <sheet name="Layer0" sheetId="79" r:id="rId3"/>
     <sheet name="Layer0 (2)" sheetId="82" r:id="rId4"/>
-    <sheet name="Layer0 (3)" sheetId="83" r:id="rId5"/>
-    <sheet name="Layer1" sheetId="81" r:id="rId6"/>
-    <sheet name="Tiles" sheetId="56" r:id="rId7"/>
+    <sheet name="Layer0 (4)" sheetId="84" r:id="rId5"/>
+    <sheet name="Layer0 (3)" sheetId="83" r:id="rId6"/>
+    <sheet name="Layer1" sheetId="81" r:id="rId7"/>
+    <sheet name="Tiles" sheetId="56" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Tiles!$C$1:$C$65</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Tiles!$C$1:$C$65</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2299" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2702" uniqueCount="275">
   <si>
     <t>width</t>
   </si>
@@ -2172,6 +2173,12 @@
   </si>
   <si>
     <t>PLAYER_THIEF</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
   <si>
     <t>#</t>
@@ -2387,7 +2394,35 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="32">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -5277,12 +5312,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="27" priority="2">
+    <cfRule type="expression" dxfId="31" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="26" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7010,12 +7045,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="25" priority="2">
+    <cfRule type="expression" dxfId="29" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="24" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7028,7 +7063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AA1" sqref="AA1:AA20"/>
     </sheetView>
   </sheetViews>
@@ -7435,19 +7470,19 @@
         <v>6</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="L6" s="12" t="s">
         <v>6</v>
@@ -7507,25 +7542,25 @@
         <v>6</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="I7" s="12" t="s">
         <v>6</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="L7" s="12" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="M7" s="12" t="s">
         <v>6</v>
@@ -7558,11 +7593,11 @@
       <c r="Y7" s="7"/>
       <c r="AA7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">     ##   ##        </v>
+        <v xml:space="preserve">     ##^ ^##        </v>
       </c>
       <c r="AB7" t="str">
         <f t="shared" si="1"/>
-        <v>'     ##   ##        ',</v>
+        <v>'     ##^ ^##        ',</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
@@ -7582,10 +7617,10 @@
         <v>6</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>6</v>
+        <v>218</v>
       </c>
       <c r="H8" s="12" t="s">
         <v>6</v>
@@ -7600,7 +7635,7 @@
         <v>6</v>
       </c>
       <c r="L8" s="12" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="M8" s="12" t="s">
         <v>6</v>
@@ -7633,11 +7668,11 @@
       <c r="Y8" s="7"/>
       <c r="AA8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">     #     #        </v>
+        <v xml:space="preserve">     #p    #        </v>
       </c>
       <c r="AB8" t="str">
         <f t="shared" si="1"/>
-        <v>'     #     #        ',</v>
+        <v>'     #p    #        ',</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -7657,7 +7692,7 @@
         <v>6</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="G9" s="12" t="s">
         <v>6</v>
@@ -7675,7 +7710,7 @@
         <v>6</v>
       </c>
       <c r="L9" s="12" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="M9" s="12" t="s">
         <v>6</v>
@@ -7732,7 +7767,7 @@
         <v>6</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>6</v>
@@ -7750,7 +7785,7 @@
         <v>6</v>
       </c>
       <c r="L10" s="12" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="M10" s="12" t="s">
         <v>6</v>
@@ -7807,25 +7842,25 @@
         <v>6</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="I11" s="12" t="s">
         <v>6</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="L11" s="12" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="M11" s="12" t="s">
         <v>6</v>
@@ -7858,11 +7893,11 @@
       <c r="Y11" s="7"/>
       <c r="AA11" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">     ##   ##        </v>
+        <v xml:space="preserve">     ##^ ^##        </v>
       </c>
       <c r="AB11" t="str">
         <f t="shared" si="1"/>
-        <v>'     ##   ##        ',</v>
+        <v>'     ##^ ^##        ',</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
@@ -7885,7 +7920,7 @@
         <v>6</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="H12" s="12" t="s">
         <v>6</v>
@@ -7897,7 +7932,7 @@
         <v>6</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="L12" s="12" t="s">
         <v>6</v>
@@ -8743,22 +8778,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="23" priority="6">
+    <cfRule type="expression" dxfId="27" priority="6">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="22" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="5" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="21" priority="4">
+    <cfRule type="expression" dxfId="25" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="20" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10486,22 +10521,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="11" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="6" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10511,11 +10546,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43DB044F-C342-48FD-9479-7EECE71FE5BB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE348DA3-3F80-4F34-AF8A-B7F24FAA7598}">
   <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1:AA20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10996,19 +11031,19 @@
         <v>6</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="L7" s="12" t="s">
         <v>6</v>
@@ -11044,11 +11079,11 @@
       <c r="Y7" s="7"/>
       <c r="AA7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">      #####         </v>
       </c>
       <c r="AB7" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>'      #####         ',</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
@@ -11071,7 +11106,7 @@
         <v>6</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="H8" s="12" t="s">
         <v>6</v>
@@ -11083,7 +11118,7 @@
         <v>6</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="L8" s="12" t="s">
         <v>6</v>
@@ -11119,11 +11154,11 @@
       <c r="Y8" s="7"/>
       <c r="AA8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">      #   #         </v>
       </c>
       <c r="AB8" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>'      #   #         ',</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -11146,7 +11181,7 @@
         <v>6</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="H9" s="12" t="s">
         <v>6</v>
@@ -11158,7 +11193,7 @@
         <v>6</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="L9" s="12" t="s">
         <v>6</v>
@@ -11194,11 +11229,11 @@
       <c r="Y9" s="7"/>
       <c r="AA9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">      #   #         </v>
       </c>
       <c r="AB9" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>'      #   #         ',</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
@@ -11218,10 +11253,10 @@
         <v>6</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="H10" s="12" t="s">
         <v>6</v>
@@ -11233,7 +11268,7 @@
         <v>6</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="L10" s="12" t="s">
         <v>6</v>
@@ -11269,11 +11304,11 @@
       <c r="Y10" s="7"/>
       <c r="AA10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">     ##   #         </v>
       </c>
       <c r="AB10" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>'     ##   #         ',</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
@@ -11293,25 +11328,25 @@
         <v>6</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="G11" s="12" t="s">
         <v>6</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>187</v>
+        <v>59</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="L11" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="M11" s="12" t="s">
         <v>6</v>
@@ -11344,11 +11379,11 @@
       <c r="Y11" s="7"/>
       <c r="AA11" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">       fff          </v>
+        <v xml:space="preserve">     # ^  ##        </v>
       </c>
       <c r="AB11" t="str">
         <f t="shared" si="1"/>
-        <v>'       fff          ',</v>
+        <v>'     # ^  ##        ',</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
@@ -11368,25 +11403,25 @@
         <v>6</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>187</v>
+        <v>59</v>
       </c>
       <c r="L12" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="M12" s="12" t="s">
         <v>6</v>
@@ -11419,11 +11454,11 @@
       <c r="Y12" s="7"/>
       <c r="AA12" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">      fffff         </v>
+        <v xml:space="preserve">     #    ^#        </v>
       </c>
       <c r="AB12" t="str">
         <f t="shared" si="1"/>
-        <v>'      fffff         ',</v>
+        <v>'     #    ^#        ',</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
@@ -11443,25 +11478,25 @@
         <v>6</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="L13" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="M13" s="12" t="s">
         <v>6</v>
@@ -11494,11 +11529,11 @@
       <c r="Y13" s="7"/>
       <c r="AA13" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">      fffff         </v>
+        <v xml:space="preserve">     #     #        </v>
       </c>
       <c r="AB13" t="str">
         <f t="shared" si="1"/>
-        <v>'      fffff         ',</v>
+        <v>'     #     #        ',</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
@@ -11518,31 +11553,31 @@
         <v>6</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>187</v>
+        <v>59</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="L14" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="M14" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="N14" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="O14" s="12" t="s">
         <v>6</v>
@@ -11569,11 +11604,11 @@
       <c r="Y14" s="7"/>
       <c r="AA14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">      fffff         </v>
+        <v xml:space="preserve">     #^    ###      </v>
       </c>
       <c r="AB14" t="str">
         <f t="shared" si="1"/>
-        <v>'      fffff         ',</v>
+        <v>'     #^    ###      ',</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
@@ -11593,31 +11628,31 @@
         <v>6</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>187</v>
+        <v>59</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="L15" s="12" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="M15" s="12" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="N15" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="O15" s="12" t="s">
         <v>6</v>
@@ -11644,11 +11679,11 @@
       <c r="Y15" s="7"/>
       <c r="AA15" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">       ffffff       </v>
+        <v xml:space="preserve">     ##  ^   #      </v>
       </c>
       <c r="AB15" t="str">
         <f t="shared" si="1"/>
-        <v>'       ffffff       ',</v>
+        <v>'     ##  ^   #      ',</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
@@ -11671,28 +11706,28 @@
         <v>6</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="L16" s="12" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="M16" s="12" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="N16" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="O16" s="12" t="s">
         <v>6</v>
@@ -11719,11 +11754,11 @@
       <c r="Y16" s="7"/>
       <c r="AA16" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">       ffffff       </v>
+        <v xml:space="preserve">      #      #      </v>
       </c>
       <c r="AB16" t="str">
         <f t="shared" si="1"/>
-        <v>'       ffffff       ',</v>
+        <v>'      #      #      ',</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
@@ -11746,28 +11781,28 @@
         <v>6</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="L17" s="12" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="M17" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="N17" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="O17" s="12" t="s">
         <v>6</v>
@@ -11794,11 +11829,11 @@
       <c r="Y17" s="7"/>
       <c r="AA17" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">         fff        </v>
+        <v xml:space="preserve">      ###   ##      </v>
       </c>
       <c r="AB17" t="str">
         <f t="shared" si="1"/>
-        <v>'         fff        ',</v>
+        <v>'      ###   ##      ',</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
@@ -11827,19 +11862,19 @@
         <v>6</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="L18" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="M18" s="12" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="N18" s="12" t="s">
         <v>6</v>
@@ -11869,11 +11904,11 @@
       <c r="Y18" s="7"/>
       <c r="AA18" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">        #####       </v>
       </c>
       <c r="AB18" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>'        #####       ',</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
@@ -12254,11 +12289,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12915BD-717D-4032-B030-25F03C2DB7C6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43DB044F-C342-48FD-9479-7EECE71FE5BB}">
   <dimension ref="A1:AB30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+      <selection activeCell="AA1" sqref="AA1:AA20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12270,65 +12305,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>272</v>
+      <c r="A1" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>272</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>272</v>
+        <v>6</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="O1" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="Q1" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>272</v>
-      </c>
-      <c r="S1" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="T1" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
@@ -12337,16 +12372,16 @@
       <c r="Y1" s="3"/>
       <c r="AA1" t="str">
         <f>CONCATENATE(A1,B1,C1,D1,E1,F1,G1,H1,I1,J1,K1,L1,M1,N1,O1,P1,Q1,R1,S1,T1,U1,V1,W1,X1,Y1)</f>
-        <v>####################</v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB1" t="str">
         <f>"'"&amp;AA1&amp;"',"</f>
-        <v>'####################',</v>
+        <v>'                    ',</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>272</v>
+      <c r="A2" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>6</v>
@@ -12403,7 +12438,7 @@
         <v>6</v>
       </c>
       <c r="T2" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="U2" s="6"/>
       <c r="V2" s="6"/>
@@ -12412,16 +12447,16 @@
       <c r="Y2" s="7"/>
       <c r="AA2" t="str">
         <f t="shared" ref="AA2:AA25" si="0">CONCATENATE(A2,B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,N2,O2,P2,Q2,R2,S2,T2,U2,V2,W2,X2,Y2)</f>
-        <v>#                  #</v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB2" t="str">
         <f t="shared" ref="AB2:AB25" si="1">"'"&amp;AA2&amp;"',"</f>
-        <v>'#                  #',</v>
+        <v>'                    ',</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>272</v>
+      <c r="A3" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>6</v>
@@ -12478,7 +12513,7 @@
         <v>6</v>
       </c>
       <c r="T3" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
@@ -12487,16 +12522,16 @@
       <c r="Y3" s="7"/>
       <c r="AA3" t="str">
         <f t="shared" si="0"/>
-        <v>#                  #</v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB3" t="str">
         <f t="shared" si="1"/>
-        <v>'#                  #',</v>
+        <v>'                    ',</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>272</v>
+      <c r="A4" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>6</v>
@@ -12553,7 +12588,7 @@
         <v>6</v>
       </c>
       <c r="T4" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
@@ -12562,16 +12597,16 @@
       <c r="Y4" s="7"/>
       <c r="AA4" t="str">
         <f t="shared" si="0"/>
-        <v>#                  #</v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB4" t="str">
         <f t="shared" si="1"/>
-        <v>'#                  #',</v>
+        <v>'                    ',</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>272</v>
+      <c r="A5" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>6</v>
@@ -12580,7 +12615,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>213</v>
+        <v>6</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>6</v>
@@ -12628,7 +12663,7 @@
         <v>6</v>
       </c>
       <c r="T5" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
@@ -12637,16 +12672,16 @@
       <c r="Y5" s="7"/>
       <c r="AA5" t="str">
         <f t="shared" si="0"/>
-        <v>#  K               #</v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB5" t="str">
         <f t="shared" si="1"/>
-        <v>'#  K               #',</v>
+        <v>'                    ',</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>272</v>
+      <c r="A6" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>6</v>
@@ -12703,7 +12738,7 @@
         <v>6</v>
       </c>
       <c r="T6" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
@@ -12712,16 +12747,16 @@
       <c r="Y6" s="7"/>
       <c r="AA6" t="str">
         <f t="shared" si="0"/>
-        <v>#                  #</v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB6" t="str">
         <f t="shared" si="1"/>
-        <v>'#                  #',</v>
+        <v>'                    ',</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>272</v>
+      <c r="A7" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>6</v>
@@ -12778,7 +12813,7 @@
         <v>6</v>
       </c>
       <c r="T7" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>
@@ -12787,16 +12822,16 @@
       <c r="Y7" s="7"/>
       <c r="AA7" t="str">
         <f t="shared" si="0"/>
-        <v>#                  #</v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB7" t="str">
         <f t="shared" si="1"/>
-        <v>'#                  #',</v>
+        <v>'                    ',</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>272</v>
+      <c r="A8" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>6</v>
@@ -12817,13 +12852,13 @@
         <v>6</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="I8" s="12" t="s">
         <v>6</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="K8" s="12" t="s">
         <v>6</v>
@@ -12853,7 +12888,7 @@
         <v>6</v>
       </c>
       <c r="T8" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="U8" s="6"/>
       <c r="V8" s="6"/>
@@ -12862,16 +12897,16 @@
       <c r="Y8" s="7"/>
       <c r="AA8" t="str">
         <f t="shared" si="0"/>
-        <v>#                  #</v>
+        <v xml:space="preserve">       O f          </v>
       </c>
       <c r="AB8" t="str">
         <f t="shared" si="1"/>
-        <v>'#                  #',</v>
+        <v>'       O f          ',</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>272</v>
+      <c r="A9" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>6</v>
@@ -12898,7 +12933,7 @@
         <v>6</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="K9" s="12" t="s">
         <v>6</v>
@@ -12928,7 +12963,7 @@
         <v>6</v>
       </c>
       <c r="T9" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="U9" s="6"/>
       <c r="V9" s="6"/>
@@ -12937,16 +12972,16 @@
       <c r="Y9" s="7"/>
       <c r="AA9" t="str">
         <f t="shared" si="0"/>
-        <v>#                  #</v>
+        <v xml:space="preserve">         f          </v>
       </c>
       <c r="AB9" t="str">
         <f t="shared" si="1"/>
-        <v>'#                  #',</v>
+        <v>'         f          ',</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>272</v>
+      <c r="A10" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>6</v>
@@ -12967,13 +13002,13 @@
         <v>6</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="K10" s="12" t="s">
         <v>6</v>
@@ -13003,7 +13038,7 @@
         <v>6</v>
       </c>
       <c r="T10" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="U10" s="6"/>
       <c r="V10" s="6"/>
@@ -13012,16 +13047,16 @@
       <c r="Y10" s="7"/>
       <c r="AA10" t="str">
         <f t="shared" si="0"/>
-        <v>#                  #</v>
+        <v xml:space="preserve">       fff          </v>
       </c>
       <c r="AB10" t="str">
         <f t="shared" si="1"/>
-        <v>'#                  #',</v>
+        <v>'       fff          ',</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>272</v>
+      <c r="A11" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>6</v>
@@ -13039,16 +13074,16 @@
         <v>6</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="K11" s="12" t="s">
         <v>6</v>
@@ -13078,7 +13113,7 @@
         <v>6</v>
       </c>
       <c r="T11" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="U11" s="6"/>
       <c r="V11" s="6"/>
@@ -13087,16 +13122,16 @@
       <c r="Y11" s="7"/>
       <c r="AA11" t="str">
         <f t="shared" si="0"/>
-        <v>#                  #</v>
+        <v xml:space="preserve">      ffff          </v>
       </c>
       <c r="AB11" t="str">
         <f t="shared" si="1"/>
-        <v>'#                  #',</v>
+        <v>'      ffff          ',</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>272</v>
+      <c r="A12" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>6</v>
@@ -13114,19 +13149,19 @@
         <v>6</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="L12" s="12" t="s">
         <v>6</v>
@@ -13153,7 +13188,7 @@
         <v>6</v>
       </c>
       <c r="T12" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="U12" s="6"/>
       <c r="V12" s="6"/>
@@ -13162,16 +13197,16 @@
       <c r="Y12" s="7"/>
       <c r="AA12" t="str">
         <f t="shared" si="0"/>
-        <v>#                  #</v>
+        <v xml:space="preserve">      fffff         </v>
       </c>
       <c r="AB12" t="str">
         <f t="shared" si="1"/>
-        <v>'#                  #',</v>
+        <v>'      fffff         ',</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>272</v>
+      <c r="A13" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>6</v>
@@ -13189,19 +13224,19 @@
         <v>6</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="L13" s="12" t="s">
         <v>6</v>
@@ -13228,7 +13263,7 @@
         <v>6</v>
       </c>
       <c r="T13" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="U13" s="6"/>
       <c r="V13" s="6"/>
@@ -13237,16 +13272,16 @@
       <c r="Y13" s="7"/>
       <c r="AA13" t="str">
         <f t="shared" si="0"/>
-        <v>#                  #</v>
+        <v xml:space="preserve">      fffff         </v>
       </c>
       <c r="AB13" t="str">
         <f t="shared" si="1"/>
-        <v>'#                  #',</v>
+        <v>'      fffff         ',</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>272</v>
+      <c r="A14" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>6</v>
@@ -13264,22 +13299,22 @@
         <v>6</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="L14" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="M14" s="12" t="s">
         <v>6</v>
@@ -13303,7 +13338,7 @@
         <v>6</v>
       </c>
       <c r="T14" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
@@ -13312,16 +13347,16 @@
       <c r="Y14" s="7"/>
       <c r="AA14" t="str">
         <f t="shared" si="0"/>
-        <v>#                  #</v>
+        <v xml:space="preserve">      ffffff        </v>
       </c>
       <c r="AB14" t="str">
         <f t="shared" si="1"/>
-        <v>'#                  #',</v>
+        <v>'      ffffff        ',</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>272</v>
+      <c r="A15" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>6</v>
@@ -13342,22 +13377,22 @@
         <v>6</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="L15" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="M15" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="N15" s="12" t="s">
         <v>6</v>
@@ -13378,7 +13413,7 @@
         <v>6</v>
       </c>
       <c r="T15" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="U15" s="6"/>
       <c r="V15" s="6"/>
@@ -13387,16 +13422,16 @@
       <c r="Y15" s="7"/>
       <c r="AA15" t="str">
         <f t="shared" si="0"/>
-        <v>#                  #</v>
+        <v xml:space="preserve">       ffffff       </v>
       </c>
       <c r="AB15" t="str">
         <f t="shared" si="1"/>
-        <v>'#                  #',</v>
+        <v>'       ffffff       ',</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>272</v>
+      <c r="A16" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>6</v>
@@ -13417,22 +13452,22 @@
         <v>6</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="L16" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="M16" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="N16" s="12" t="s">
         <v>6</v>
@@ -13441,7 +13476,7 @@
         <v>6</v>
       </c>
       <c r="P16" s="12" t="s">
-        <v>213</v>
+        <v>6</v>
       </c>
       <c r="Q16" s="12" t="s">
         <v>6</v>
@@ -13453,7 +13488,7 @@
         <v>6</v>
       </c>
       <c r="T16" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="U16" s="6"/>
       <c r="V16" s="6"/>
@@ -13462,16 +13497,16 @@
       <c r="Y16" s="7"/>
       <c r="AA16" t="str">
         <f t="shared" si="0"/>
-        <v>#              K   #</v>
+        <v xml:space="preserve">       ffffff       </v>
       </c>
       <c r="AB16" t="str">
         <f t="shared" si="1"/>
-        <v>'#              K   #',</v>
+        <v>'       ffffff       ',</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>272</v>
+      <c r="A17" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>6</v>
@@ -13498,13 +13533,13 @@
         <v>6</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="L17" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="M17" s="12" t="s">
         <v>6</v>
@@ -13528,7 +13563,7 @@
         <v>6</v>
       </c>
       <c r="T17" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="U17" s="6"/>
       <c r="V17" s="6"/>
@@ -13537,16 +13572,16 @@
       <c r="Y17" s="7"/>
       <c r="AA17" t="str">
         <f t="shared" si="0"/>
-        <v>#                  #</v>
+        <v xml:space="preserve">         fff        </v>
       </c>
       <c r="AB17" t="str">
         <f t="shared" si="1"/>
-        <v>'#                  #',</v>
+        <v>'         fff        ',</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>272</v>
+      <c r="A18" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>6</v>
@@ -13603,7 +13638,7 @@
         <v>6</v>
       </c>
       <c r="T18" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
@@ -13612,16 +13647,16 @@
       <c r="Y18" s="7"/>
       <c r="AA18" t="str">
         <f t="shared" si="0"/>
-        <v>#                  #</v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB18" t="str">
         <f t="shared" si="1"/>
-        <v>'#                  #',</v>
+        <v>'                    ',</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>272</v>
+      <c r="A19" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>6</v>
@@ -13678,7 +13713,7 @@
         <v>6</v>
       </c>
       <c r="T19" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="U19" s="6"/>
       <c r="V19" s="6"/>
@@ -13687,73 +13722,73 @@
       <c r="Y19" s="7"/>
       <c r="AA19" t="str">
         <f t="shared" si="0"/>
-        <v>#                  #</v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB19" t="str">
         <f t="shared" si="1"/>
-        <v>'#                  #',</v>
+        <v>'                    ',</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>272</v>
+      <c r="A20" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="L20" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="M20" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="N20" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="O20" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="P20" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="Q20" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="R20" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="S20" s="5" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="T20" s="12" t="s">
-        <v>272</v>
+        <v>6</v>
       </c>
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
@@ -13762,11 +13797,11 @@
       <c r="Y20" s="7"/>
       <c r="AA20" t="str">
         <f t="shared" si="0"/>
-        <v>####################</v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB20" t="str">
         <f t="shared" si="1"/>
-        <v>'####################',</v>
+        <v>'                    ',</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
@@ -13972,32 +14007,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="13" priority="6">
+    <cfRule type="expression" dxfId="7" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="12" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:T2 A3:A18 T3:T18 B3:S19">
-    <cfRule type="expression" dxfId="11" priority="4">
+  <conditionalFormatting sqref="A1:T20">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:T2 A3:A18 T3:T18 B3:S19">
-    <cfRule type="cellIs" dxfId="10" priority="3" stopIfTrue="1" operator="equal">
-      <formula>":"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A20:T20 A19 T19">
-    <cfRule type="expression" dxfId="9" priority="2">
-      <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A20:T20 A19 T19">
-    <cfRule type="cellIs" dxfId="8" priority="1" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="A1:T20">
+    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14007,6 +14032,1757 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12915BD-717D-4032-B030-25F03C2DB7C6}">
+  <dimension ref="A1:AB30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1:AA20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="T1" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="3"/>
+      <c r="AA1" t="str">
+        <f>CONCATENATE(A1,B1,C1,D1,E1,F1,G1,H1,I1,J1,K1,L1,M1,N1,O1,P1,Q1,R1,S1,T1,U1,V1,W1,X1,Y1)</f>
+        <v>####################</v>
+      </c>
+      <c r="AB1" t="str">
+        <f>"'"&amp;AA1&amp;"',"</f>
+        <v>'####################',</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="R2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="7"/>
+      <c r="AA2" t="str">
+        <f t="shared" ref="AA2:AA25" si="0">CONCATENATE(A2,B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,N2,O2,P2,Q2,R2,S2,T2,U2,V2,W2,X2,Y2)</f>
+        <v>#+   ##           ^#</v>
+      </c>
+      <c r="AB2" t="str">
+        <f t="shared" ref="AB2:AB25" si="1">"'"&amp;AA2&amp;"',"</f>
+        <v>'#+   ##           ^#',</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="R3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="T3" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="7"/>
+      <c r="AA3" t="str">
+        <f t="shared" si="0"/>
+        <v>#                 k#</v>
+      </c>
+      <c r="AB3" t="str">
+        <f t="shared" si="1"/>
+        <v>'#                 k#',</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="P4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="R4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="T4" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="7"/>
+      <c r="AA4" t="str">
+        <f t="shared" si="0"/>
+        <v>#                  #</v>
+      </c>
+      <c r="AB4" t="str">
+        <f t="shared" si="1"/>
+        <v>'#                  #',</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="P5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="R5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="T5" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="7"/>
+      <c r="AA5" t="str">
+        <f t="shared" si="0"/>
+        <v>#    ##     $      #</v>
+      </c>
+      <c r="AB5" t="str">
+        <f t="shared" si="1"/>
+        <v>'#    ##     $      #',</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="P6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="R6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="T6" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="7"/>
+      <c r="AA6" t="str">
+        <f t="shared" si="0"/>
+        <v>######             #</v>
+      </c>
+      <c r="AB6" t="str">
+        <f t="shared" si="1"/>
+        <v>'######             #',</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="O7" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="P7" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="R7" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="S7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="T7" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="7"/>
+      <c r="AA7" t="str">
+        <f t="shared" si="0"/>
+        <v>######             #</v>
+      </c>
+      <c r="AB7" t="str">
+        <f t="shared" si="1"/>
+        <v>'######             #',</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="N8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="O8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="R8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="T8" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="7"/>
+      <c r="AA8" t="str">
+        <f t="shared" si="0"/>
+        <v>#    #   #         #</v>
+      </c>
+      <c r="AB8" t="str">
+        <f t="shared" si="1"/>
+        <v>'#    #   #         #',</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="N9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="O9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="P9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="R9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="S9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="T9" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="7"/>
+      <c r="AA9" t="str">
+        <f t="shared" si="0"/>
+        <v>#    #####         #</v>
+      </c>
+      <c r="AB9" t="str">
+        <f t="shared" si="1"/>
+        <v>'#    #####         #',</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="O10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="P10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="R10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="S10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="T10" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="7"/>
+      <c r="AA10" t="str">
+        <f t="shared" si="0"/>
+        <v>#  ^     #  $      #</v>
+      </c>
+      <c r="AB10" t="str">
+        <f t="shared" si="1"/>
+        <v>'#  ^     #  $      #',</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="N11" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="O11" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="P11" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q11" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="R11" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="S11" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="T11" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="7"/>
+      <c r="AA11" t="str">
+        <f t="shared" si="0"/>
+        <v># ^K^             ##</v>
+      </c>
+      <c r="AB11" t="str">
+        <f t="shared" si="1"/>
+        <v>'# ^K^             ##',</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="N12" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="O12" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="P12" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q12" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="R12" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="S12" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="T12" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="7"/>
+      <c r="AA12" t="str">
+        <f t="shared" si="0"/>
+        <v>#            #######</v>
+      </c>
+      <c r="AB12" t="str">
+        <f t="shared" si="1"/>
+        <v>'#            #######',</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M13" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="N13" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="O13" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="P13" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q13" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="R13" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="S13" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="T13" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="6"/>
+      <c r="Y13" s="7"/>
+      <c r="AA13" t="str">
+        <f t="shared" si="0"/>
+        <v>#            #    ##</v>
+      </c>
+      <c r="AB13" t="str">
+        <f t="shared" si="1"/>
+        <v>'#            #    ##',</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="N14" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="O14" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="P14" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q14" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="R14" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="S14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="T14" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="6"/>
+      <c r="Y14" s="7"/>
+      <c r="AA14" t="str">
+        <f t="shared" si="0"/>
+        <v>#            #     #</v>
+      </c>
+      <c r="AB14" t="str">
+        <f t="shared" si="1"/>
+        <v>'#            #     #',</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L15" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M15" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="N15" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="O15" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="P15" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q15" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="R15" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="S15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="T15" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="7"/>
+      <c r="AA15" t="str">
+        <f t="shared" si="0"/>
+        <v>#      $       ^   #</v>
+      </c>
+      <c r="AB15" t="str">
+        <f t="shared" si="1"/>
+        <v>'#      $       ^   #',</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="N16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="O16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="P16" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q16" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="R16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="S16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="T16" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="7"/>
+      <c r="AA16" t="str">
+        <f t="shared" si="0"/>
+        <v>#              K^  #</v>
+      </c>
+      <c r="AB16" t="str">
+        <f t="shared" si="1"/>
+        <v>'#              K^  #',</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="N17" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="O17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="P17" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="R17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="S17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="T17" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="6"/>
+      <c r="Y17" s="7"/>
+      <c r="AA17" t="str">
+        <f t="shared" si="0"/>
+        <v>#            # ^   #</v>
+      </c>
+      <c r="AB17" t="str">
+        <f t="shared" si="1"/>
+        <v>'#            # ^   #',</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="N18" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="O18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="P18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="R18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="S18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="T18" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="6"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="7"/>
+      <c r="AA18" t="str">
+        <f t="shared" si="0"/>
+        <v>#n           #     #</v>
+      </c>
+      <c r="AB18" t="str">
+        <f t="shared" si="1"/>
+        <v>'#n           #     #',</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K19" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L19" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M19" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="N19" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="O19" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="P19" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q19" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="R19" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="S19" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="T19" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="U19" s="6"/>
+      <c r="V19" s="6"/>
+      <c r="W19" s="6"/>
+      <c r="X19" s="6"/>
+      <c r="Y19" s="7"/>
+      <c r="AA19" t="str">
+        <f t="shared" si="0"/>
+        <v>#          ###   ^#</v>
+      </c>
+      <c r="AB19" t="str">
+        <f t="shared" si="1"/>
+        <v>'#          ###   ^#',</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="K20" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="L20" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="M20" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="N20" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="O20" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="P20" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q20" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="R20" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="S20" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="T20" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="U20" s="6"/>
+      <c r="V20" s="6"/>
+      <c r="W20" s="6"/>
+      <c r="X20" s="6"/>
+      <c r="Y20" s="7"/>
+      <c r="AA20" t="str">
+        <f t="shared" si="0"/>
+        <v>####################</v>
+      </c>
+      <c r="AB20" t="str">
+        <f t="shared" si="1"/>
+        <v>'####################',</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+      <c r="X21" s="6"/>
+      <c r="Y21" s="7"/>
+      <c r="AA21" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AB21" t="str">
+        <f t="shared" si="1"/>
+        <v>'',</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="5"/>
+      <c r="U22" s="6"/>
+      <c r="V22" s="6"/>
+      <c r="W22" s="6"/>
+      <c r="X22" s="6"/>
+      <c r="Y22" s="7"/>
+      <c r="AA22" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AB22" t="str">
+        <f t="shared" si="1"/>
+        <v>'',</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="5"/>
+      <c r="T23" s="5"/>
+      <c r="U23" s="6"/>
+      <c r="V23" s="6"/>
+      <c r="W23" s="6"/>
+      <c r="X23" s="6"/>
+      <c r="Y23" s="7"/>
+      <c r="AA23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AB23" t="str">
+        <f t="shared" si="1"/>
+        <v>'',</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="5"/>
+      <c r="T24" s="5"/>
+      <c r="U24" s="6"/>
+      <c r="V24" s="6"/>
+      <c r="W24" s="6"/>
+      <c r="X24" s="6"/>
+      <c r="Y24" s="7"/>
+      <c r="AA24" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AB24" t="str">
+        <f t="shared" si="1"/>
+        <v>'',</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="8"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="10"/>
+      <c r="V25" s="10"/>
+      <c r="W25" s="10"/>
+      <c r="X25" s="10"/>
+      <c r="Y25" s="11"/>
+      <c r="AA25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AB25" t="str">
+        <f t="shared" si="1"/>
+        <v>'',</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A21:Y25 U1:Y20">
+    <cfRule type="expression" dxfId="17" priority="6">
+      <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21:Z25 U1:Z20">
+    <cfRule type="cellIs" dxfId="16" priority="5" stopIfTrue="1" operator="equal">
+      <formula>":"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:T2 A3:A18 T3:T18 B3:S19">
+    <cfRule type="expression" dxfId="15" priority="4">
+      <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:T2 A3:A18 T3:T18 B3:S19">
+    <cfRule type="cellIs" dxfId="14" priority="3" stopIfTrue="1" operator="equal">
+      <formula>":"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20:T20 A19 T19">
+    <cfRule type="expression" dxfId="13" priority="2">
+      <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20:T20 A19 T19">
+    <cfRule type="cellIs" dxfId="12" priority="1" stopIfTrue="1" operator="equal">
+      <formula>":"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:K77"/>
   <sheetViews>
@@ -16411,22 +18187,22 @@
     <sortCondition ref="B2:B67"/>
   </sortState>
   <conditionalFormatting sqref="D1:D31 D33:D1048576">
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="4" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K31 K33:K77">
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
wrapped up level 110
</commit_message>
<xml_diff>
--- a/darkworld/model/data/floor builder 20200330.xlsx
+++ b/darkworld/model/data/floor builder 20200330.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Development\Python\DarkWorld\darkworld\model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BC69E9-6FBA-4274-B107-9CF507B3F4ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB946B4-A8C2-458B-9839-C6086D54D81B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12555" yWindow="2715" windowWidth="25065" windowHeight="15840" tabRatio="904" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13020" yWindow="4680" windowWidth="25065" windowHeight="15840" tabRatio="904" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blank" sheetId="49" r:id="rId1"/>
@@ -16022,8 +16022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43DB044F-C342-48FD-9479-7EECE71FE5BB}">
   <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1:AA20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16582,10 +16582,10 @@
         <v>4</v>
       </c>
       <c r="H8" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="12" t="s">
         <v>11</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>4</v>
       </c>
       <c r="J8" s="12" t="s">
         <v>54</v>
@@ -16627,11 +16627,11 @@
       <c r="Y8" s="7"/>
       <c r="AA8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">       O f          </v>
+        <v xml:space="preserve">       fOf          </v>
       </c>
       <c r="AB8" t="str">
         <f t="shared" si="1"/>
-        <v>'       O f          ',</v>
+        <v>'       fOf          ',</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -16657,10 +16657,10 @@
         <v>4</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="J9" s="12" t="s">
         <v>54</v>
@@ -16702,11 +16702,11 @@
       <c r="Y9" s="7"/>
       <c r="AA9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">         f          </v>
+        <v xml:space="preserve">       fff          </v>
       </c>
       <c r="AB9" t="str">
         <f t="shared" si="1"/>
-        <v>'         f          ',</v>
+        <v>'       fff          ',</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
@@ -17765,7 +17765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD870BA-468A-4F81-B3CE-2FB1001B4462}">
   <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA1" sqref="AA1:AA20"/>
     </sheetView>
   </sheetViews>

</xml_diff>